<commit_message>
Fix DataField.BaseField index determination. Should be relative to source range's first column.
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Other/PivotTableReferenceFiles/TwoPivotTablesWithSingleSource/output.xlsx
+++ b/ClosedXML_Tests/Resource/Other/PivotTableReferenceFiles/TwoPivotTablesWithSingleSource/output.xlsx
@@ -1602,8 +1602,8 @@
 <x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" itemPrintTitles="1" mergeItem="1" indent="0" compact="0" compactData="0" gridDropZones="1">
   <x:location ref="B3" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <x:pivotFields count="7">
-    <x:pivotField name="Company" axis="axisRow" compact="0" outline="0" showAll="0" includeNewItemsInFilter="1" defaultSubtotal="0">
-      <x:items count="54">
+    <x:pivotField name="Company" axis="axisRow" compact="0" outline="0" showAll="0" includeNewItemsInFilter="1">
+      <x:items count="55">
         <x:item x="0"/>
         <x:item x="1"/>
         <x:item x="2"/>
@@ -1658,10 +1658,11 @@
         <x:item x="51"/>
         <x:item x="52"/>
         <x:item x="53"/>
+        <x:item t="default"/>
       </x:items>
     </x:pivotField>
-    <x:pivotField name="Payment method" axis="axisRow" compact="0" outline="0" showAll="0" includeNewItemsInFilter="1" defaultSubtotal="0">
-      <x:items count="7">
+    <x:pivotField name="Payment method" axis="axisRow" compact="0" outline="0" showAll="0" includeNewItemsInFilter="1">
+      <x:items count="8">
         <x:item x="0"/>
         <x:item x="1"/>
         <x:item x="2"/>
@@ -1669,10 +1670,11 @@
         <x:item x="4"/>
         <x:item x="5"/>
         <x:item x="6"/>
+        <x:item t="default"/>
       </x:items>
     </x:pivotField>
-    <x:pivotField name="OrderNo" axis="axisRow" compact="0" outline="0" showAll="0" includeNewItemsInFilter="1" defaultSubtotal="0">
-      <x:items count="205">
+    <x:pivotField name="OrderNo" axis="axisRow" compact="0" outline="0" showAll="0" includeNewItemsInFilter="1">
+      <x:items count="206">
         <x:item x="0"/>
         <x:item x="1"/>
         <x:item x="2"/>
@@ -1878,18 +1880,32 @@
         <x:item x="202"/>
         <x:item x="203"/>
         <x:item x="204"/>
+        <x:item t="default"/>
       </x:items>
     </x:pivotField>
-    <x:pivotField name="Ship date" compact="0" outline="0" defaultSubtotal="0"/>
-    <x:pivotField name="Items total" dataField="1" compact="0" outline="0" defaultSubtotal="0"/>
-    <x:pivotField name="Tax rate" axis="axisCol" compact="0" outline="0" showAll="0" includeNewItemsInFilter="1" defaultSubtotal="0">
-      <x:items count="3">
+    <x:pivotField name="Ship date" compact="0" outline="0">
+      <x:items count="1">
+        <x:item t="default"/>
+      </x:items>
+    </x:pivotField>
+    <x:pivotField name="Items total" dataField="1" compact="0" outline="0">
+      <x:items count="1">
+        <x:item t="default"/>
+      </x:items>
+    </x:pivotField>
+    <x:pivotField name="Tax rate" axis="axisCol" compact="0" outline="0" showAll="0" includeNewItemsInFilter="1">
+      <x:items count="4">
         <x:item x="0"/>
         <x:item x="1"/>
         <x:item x="2"/>
+        <x:item t="default"/>
       </x:items>
     </x:pivotField>
-    <x:pivotField name="Amount paid" dataField="1" compact="0" outline="0" defaultSubtotal="0"/>
+    <x:pivotField name="Amount paid" dataField="1" compact="0" outline="0">
+      <x:items count="1">
+        <x:item t="default"/>
+      </x:items>
+    </x:pivotField>
   </x:pivotFields>
   <x:rowFields count="3">
     <x:field x="0"/>
@@ -2724,8 +2740,8 @@
     </x:i>
   </x:colItems>
   <x:dataFields count="2">
-    <x:dataField name="Sum Amount paid" fld="6" subtotal="sum" showDataAs="normal" baseField="1" baseItem="0" numFmtId="0"/>
-    <x:dataField name="Sum Items total" fld="4" subtotal="sum" showDataAs="normal" baseField="1" baseItem="0" numFmtId="0"/>
+    <x:dataField name="Sum Amount paid" fld="6" subtotal="sum" showDataAs="normal" baseField="0" baseItem="0" numFmtId="0"/>
+    <x:dataField name="Sum Items total" fld="4" subtotal="sum" showDataAs="normal" baseField="0" baseItem="0" numFmtId="0"/>
   </x:dataFields>
   <x:formats count="1">
     <x:format dxfId="1">
@@ -2749,8 +2765,8 @@
 <x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="0" dataCaption="Values" showError="0" missingCaption="" showMissing="1" useAutoFormatting="1" pageWrap="0" pageOverThenDown="0" itemPrintTitles="1" mergeItem="1" indent="0" compact="0" compactData="0" gridDropZones="1">
   <x:location ref="B4" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <x:pivotFields count="7">
-    <x:pivotField name="Company" axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <x:items count="54">
+    <x:pivotField name="Company" axis="axisRow" compact="0" outline="0" showAll="0">
+      <x:items count="55">
         <x:item x="0"/>
         <x:item x="1"/>
         <x:item x="2"/>
@@ -2805,10 +2821,11 @@
         <x:item x="51"/>
         <x:item x="52"/>
         <x:item x="53"/>
+        <x:item t="default"/>
       </x:items>
     </x:pivotField>
-    <x:pivotField name="Payment method" axis="axisCol" compact="0" outline="0" showAll="0" includeNewItemsInFilter="1" defaultSubtotal="0">
-      <x:items count="7">
+    <x:pivotField name="Payment method" axis="axisCol" compact="0" outline="0" showAll="0" includeNewItemsInFilter="1">
+      <x:items count="8">
         <x:item x="0"/>
         <x:item x="1"/>
         <x:item x="2"/>
@@ -2816,10 +2833,11 @@
         <x:item x="4"/>
         <x:item x="5"/>
         <x:item x="6"/>
+        <x:item t="default"/>
       </x:items>
     </x:pivotField>
-    <x:pivotField name="OrderNo" axis="axisRow" compact="0" outline="0" showAll="0" includeNewItemsInFilter="1" defaultSubtotal="0">
-      <x:items count="205">
+    <x:pivotField name="OrderNo" axis="axisRow" compact="0" outline="0" showAll="0" includeNewItemsInFilter="1">
+      <x:items count="206">
         <x:item x="0"/>
         <x:item x="1"/>
         <x:item x="2"/>
@@ -3025,12 +3043,29 @@
         <x:item x="202"/>
         <x:item x="203"/>
         <x:item x="204"/>
+        <x:item t="default"/>
       </x:items>
     </x:pivotField>
-    <x:pivotField name="Ship date" compact="0" outline="0" defaultSubtotal="0"/>
-    <x:pivotField name="Items total" dataField="1" compact="0" outline="0" defaultSubtotal="0"/>
-    <x:pivotField name="Tax rate" compact="0" outline="0" defaultSubtotal="0"/>
-    <x:pivotField name="Amount paid" compact="0" outline="0" defaultSubtotal="0"/>
+    <x:pivotField name="Ship date" compact="0" outline="0">
+      <x:items count="1">
+        <x:item t="default"/>
+      </x:items>
+    </x:pivotField>
+    <x:pivotField name="Items total" dataField="1" compact="0" outline="0">
+      <x:items count="1">
+        <x:item t="default"/>
+      </x:items>
+    </x:pivotField>
+    <x:pivotField name="Tax rate" compact="0" outline="0">
+      <x:items count="1">
+        <x:item t="default"/>
+      </x:items>
+    </x:pivotField>
+    <x:pivotField name="Amount paid" compact="0" outline="0">
+      <x:items count="1">
+        <x:item t="default"/>
+      </x:items>
+    </x:pivotField>
   </x:pivotFields>
   <x:rowFields count="2">
     <x:field x="0"/>
@@ -3851,7 +3886,7 @@
     </x:i>
   </x:colItems>
   <x:dataFields count="1">
-    <x:dataField name="Sum of Items total" fld="4" subtotal="sum" showDataAs="normal" baseField="1" baseItem="0" numFmtId="0"/>
+    <x:dataField name="Sum of Items total" fld="4" subtotal="sum" showDataAs="normal" baseField="0" baseItem="0" numFmtId="0"/>
   </x:dataFields>
   <x:formats count="1">
     <x:format dxfId="1">

</xml_diff>